<commit_message>
"Line and Branch Coverage for contains()"
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\Desktop\Mestrado\Verificação e Validação de Software\vvs_2324_assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF0FF9B-EE06-435D-962A-04DA2BF3A9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7EFFE4-ECAE-4D31-856E-2A0AEE3B5C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F9D7C08-C461-4BDB-AD69-3CC85B7B7B95}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Test Case</t>
   </si>
@@ -128,6 +128,54 @@
   </si>
   <si>
     <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>[1,2,3][1,2,3]
+ Same Object</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>1,3,4</t>
+  </si>
+  <si>
+    <t>B1!,B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1:[2][3:[12:[13][34]][49:[55:[67]][77]]]]
+Input: 34
+</t>
+  </si>
+  <si>
+    <t>B1!,B2!,B3!,B4,B5
+B6,B7,B8</t>
+  </si>
+  <si>
+    <t>1,3,5,8,9,10,
+11,12,13,14,15,
+16,17,18,19,20,
+21</t>
+  </si>
+  <si>
+    <t>[1:[2][3]]
+Input: 1</t>
+  </si>
+  <si>
+    <t>[], Input: 1</t>
+  </si>
+  <si>
+    <t>[1]
+Input: 1</t>
+  </si>
+  <si>
+    <t>1,3,5,6</t>
+  </si>
+  <si>
+    <t>B1!,B2!,B3</t>
   </si>
 </sst>
 </file>
@@ -169,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -180,29 +228,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,16 +574,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33542FD-06D6-4612-B725-39F18BB506C8}">
-  <dimension ref="F4:L9"/>
+  <dimension ref="F4:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="7" max="7" width="32.21875" customWidth="1"/>
     <col min="8" max="8" width="15.109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.21875" customWidth="1"/>
     <col min="10" max="10" width="16.109375" customWidth="1"/>
@@ -556,125 +592,125 @@
   </cols>
   <sheetData>
     <row r="4" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="G4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="H5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="4">
-        <v>1</v>
-      </c>
-      <c r="L5" s="4" t="s">
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="6:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="6" t="b">
+      <c r="H6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="6" t="b">
+      <c r="I6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="6:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="6" t="s">
+      <c r="H7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="6:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="6:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="2" t="b">
@@ -683,7 +719,7 @@
       <c r="I9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K9" s="2">
@@ -691,6 +727,147 @@
       </c>
       <c r="L9" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="6:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="L11" s="2"/>
+    </row>
+    <row r="28" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="6:12" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="6:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="6:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="F32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>